<commit_message>
Atualizao Plnilhas de CheckList e Planejamento
</commit_message>
<xml_diff>
--- a/SGB/6.Gerenciamento de Projeto/SGB - Checklist Verificacao de Projeto.xlsx
+++ b/SGB/6.Gerenciamento de Projeto/SGB - Checklist Verificacao de Projeto.xlsx
@@ -181,7 +181,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="118">
   <si>
     <t>IAP - Indicador de Aderência ao Processo (70% a 100%)</t>
   </si>
@@ -982,8 +982,8 @@
     <xf borderId="3" fillId="4" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf borderId="3" fillId="5" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="3" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="3" fillId="5" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -1039,11 +1039,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="686406266"/>
-        <c:axId val="1985699846"/>
+        <c:axId val="1668959565"/>
+        <c:axId val="1862376021"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="686406266"/>
+        <c:axId val="1668959565"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1095,10 +1095,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1985699846"/>
+        <c:crossAx val="1862376021"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1985699846"/>
+        <c:axId val="1862376021"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1162,7 +1162,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="686406266"/>
+        <c:crossAx val="1668959565"/>
       </c:valAx>
     </c:plotArea>
     <c:plotVisOnly val="1"/>
@@ -1317,11 +1317,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="2019800134"/>
-        <c:axId val="67421991"/>
+        <c:axId val="601022044"/>
+        <c:axId val="1804069616"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2019800134"/>
+        <c:axId val="601022044"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1373,10 +1373,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="67421991"/>
+        <c:crossAx val="1804069616"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="67421991"/>
+        <c:axId val="1804069616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1440,7 +1440,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2019800134"/>
+        <c:crossAx val="601022044"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -1613,11 +1613,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="183336213"/>
-        <c:axId val="737200568"/>
+        <c:axId val="1513498537"/>
+        <c:axId val="1103392663"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="183336213"/>
+        <c:axId val="1513498537"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1669,10 +1669,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="737200568"/>
+        <c:crossAx val="1103392663"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="737200568"/>
+        <c:axId val="1103392663"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1736,7 +1736,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="183336213"/>
+        <c:crossAx val="1513498537"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -1877,11 +1877,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="306843621"/>
-        <c:axId val="516692855"/>
+        <c:axId val="1208127549"/>
+        <c:axId val="1958892859"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="306843621"/>
+        <c:axId val="1208127549"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1933,10 +1933,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="516692855"/>
+        <c:crossAx val="1958892859"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="516692855"/>
+        <c:axId val="1958892859"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1948,7 +1948,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="306843621"/>
+        <c:crossAx val="1208127549"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -2089,11 +2089,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="1385524051"/>
-        <c:axId val="1140647480"/>
+        <c:axId val="558453604"/>
+        <c:axId val="1506973131"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1385524051"/>
+        <c:axId val="558453604"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2145,10 +2145,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1140647480"/>
+        <c:crossAx val="1506973131"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1140647480"/>
+        <c:axId val="1506973131"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2160,7 +2160,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="1385524051"/>
+        <c:crossAx val="558453604"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -2575,7 +2575,7 @@
       </c>
       <c r="B4" s="5">
         <f>'Ver-Elaboração1'!$F$2</f>
-        <v>0.9</v>
+        <v>0.7727272727</v>
       </c>
     </row>
     <row r="5">
@@ -5864,21 +5864,21 @@
       <c r="N7" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="O7" s="8" t="str">
+      <c r="O7" s="8">
         <f>('Ver-Elaboração1'!$G$18/SUM('Ver-Elaboração1'!$G$18:'Ver-Elaboração1'!$J$18))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P7" s="8" t="str">
+        <v>0.5</v>
+      </c>
+      <c r="P7" s="8">
         <f>('Ver-Elaboração1'!$H$18/SUM('Ver-Elaboração1'!$G$18:'Ver-Elaboração1'!$J$18))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q7" s="8" t="str">
+        <v>0.5</v>
+      </c>
+      <c r="Q7" s="8">
         <f>('Ver-Elaboração1'!$I$18/SUM('Ver-Elaboração1'!$G$18:'Ver-Elaboração1'!$J$18))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R7" s="8" t="str">
+        <v>0</v>
+      </c>
+      <c r="R7" s="8">
         <f>('Ver-Elaboração1'!$J$18/SUM('Ver-Elaboração1'!$G$18:'Ver-Elaboração1'!$J$18))</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8">
@@ -5946,7 +5946,7 @@
       </c>
       <c r="O9" s="8">
         <f>('Ver-Elaboração1'!$G$23/SUM('Ver-Elaboração1'!$G$23:'Ver-Elaboração1'!$J$23))</f>
-        <v>1</v>
+        <v>0.6</v>
       </c>
       <c r="P9" s="8">
         <f>('Ver-Elaboração1'!$H$23/SUM('Ver-Elaboração1'!$G$23:'Ver-Elaboração1'!$J$23))</f>
@@ -5958,7 +5958,7 @@
       </c>
       <c r="R9" s="8">
         <f>('Ver-Elaboração1'!$J$23/SUM('Ver-Elaboração1'!$G$23:'Ver-Elaboração1'!$J$23))</f>
-        <v>0</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="10">
@@ -5986,11 +5986,11 @@
       </c>
       <c r="O10" s="8">
         <f>('Ver-Elaboração1'!$G$29/SUM('Ver-Elaboração1'!$G$29:'Ver-Elaboração1'!$J$29))</f>
-        <v>0.5</v>
+        <v>0.6666666667</v>
       </c>
       <c r="P10" s="8">
         <f>('Ver-Elaboração1'!$H$29/SUM('Ver-Elaboração1'!$G$29:'Ver-Elaboração1'!$J$29))</f>
-        <v>0.5</v>
+        <v>0.3333333333</v>
       </c>
       <c r="Q10" s="8">
         <f>('Ver-Elaboração1'!$I$29/SUM('Ver-Elaboração1'!$G$29:'Ver-Elaboração1'!$J$29))</f>
@@ -6024,21 +6024,21 @@
       <c r="N11" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="O11" s="8" t="str">
+      <c r="O11" s="8">
         <f>('Ver-Elaboração1'!$G$36/SUM('Ver-Elaboração1'!$G$36:'Ver-Elaboração1'!$J$36))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P11" s="8" t="str">
+        <v>0.6666666667</v>
+      </c>
+      <c r="P11" s="8">
         <f>('Ver-Elaboração1'!$H$36/SUM('Ver-Elaboração1'!$G$36:'Ver-Elaboração1'!$J$36))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q11" s="8" t="str">
+        <v>0.3333333333</v>
+      </c>
+      <c r="Q11" s="8">
         <f>('Ver-Elaboração1'!$I$36/SUM('Ver-Elaboração1'!$G$36:'Ver-Elaboração1'!$J$36))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R11" s="8" t="str">
+        <v>0</v>
+      </c>
+      <c r="R11" s="8">
         <f>('Ver-Elaboração1'!$J$36/SUM('Ver-Elaboração1'!$G$36:'Ver-Elaboração1'!$J$36))</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12">
@@ -6064,21 +6064,21 @@
       <c r="N12" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="O12" s="8" t="str">
+      <c r="O12" s="8">
         <f>('Ver-Elaboração1'!$G$40/SUM('Ver-Elaboração1'!$G$40:'Ver-Elaboração1'!$J$40))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P12" s="8" t="str">
+        <v>0</v>
+      </c>
+      <c r="P12" s="8">
         <f>('Ver-Elaboração1'!$H$40/SUM('Ver-Elaboração1'!$G$40:'Ver-Elaboração1'!$J$40))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q12" s="8" t="str">
+        <v>0</v>
+      </c>
+      <c r="Q12" s="8">
         <f>('Ver-Elaboração1'!$I$40/SUM('Ver-Elaboração1'!$G$40:'Ver-Elaboração1'!$J$40))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R12" s="8" t="str">
+        <v>0</v>
+      </c>
+      <c r="R12" s="8">
         <f>('Ver-Elaboração1'!$J$40/SUM('Ver-Elaboração1'!$G$40:'Ver-Elaboração1'!$J$40))</f>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1"/>
@@ -12296,7 +12296,7 @@
       <c r="E2" s="15"/>
       <c r="F2" s="16">
         <f>COUNTIF(D5:D41,"Sim")/(COUNTA(D5:D42)-COUNTIF(D5:D42,"NA"))</f>
-        <v>0.9</v>
+        <v>0.7727272727</v>
       </c>
     </row>
     <row r="3" ht="18.75" customHeight="1">
@@ -12437,7 +12437,9 @@
       <c r="C9" s="30" t="s">
         <v>75</v>
       </c>
-      <c r="D9" s="48"/>
+      <c r="D9" s="31" t="s">
+        <v>46</v>
+      </c>
       <c r="E9" s="30"/>
       <c r="F9" s="30"/>
       <c r="K9" s="35"/>
@@ -12587,7 +12589,7 @@
       <c r="C17" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="D17" s="49"/>
+      <c r="D17" s="48"/>
       <c r="E17" s="27"/>
       <c r="F17" s="27"/>
     </row>
@@ -12599,16 +12601,18 @@
       <c r="C18" s="30" t="s">
         <v>82</v>
       </c>
-      <c r="D18" s="48"/>
+      <c r="D18" s="31" t="s">
+        <v>46</v>
+      </c>
       <c r="E18" s="30"/>
       <c r="F18" s="30"/>
       <c r="G18" s="7">
         <f>COUNTIF(D18:D21,"Sim")</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H18" s="7">
         <f>COUNTIF(D18:D21,"Parcialmente")</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I18" s="7">
         <f>COUNTIF(D18:D21,"Não")</f>
@@ -12627,7 +12631,9 @@
       <c r="C19" s="34" t="s">
         <v>83</v>
       </c>
-      <c r="D19" s="48"/>
+      <c r="D19" s="31" t="s">
+        <v>72</v>
+      </c>
       <c r="E19" s="30"/>
       <c r="F19" s="30"/>
     </row>
@@ -12639,7 +12645,9 @@
       <c r="C20" s="30" t="s">
         <v>84</v>
       </c>
-      <c r="D20" s="48"/>
+      <c r="D20" s="31" t="s">
+        <v>72</v>
+      </c>
       <c r="E20" s="30"/>
       <c r="F20" s="30"/>
       <c r="G20" s="35"/>
@@ -12671,7 +12679,9 @@
       <c r="C21" s="30" t="s">
         <v>85</v>
       </c>
-      <c r="D21" s="48"/>
+      <c r="D21" s="31" t="s">
+        <v>46</v>
+      </c>
       <c r="E21" s="30"/>
       <c r="F21" s="30"/>
     </row>
@@ -12683,7 +12693,7 @@
       <c r="C22" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="D22" s="49"/>
+      <c r="D22" s="48"/>
       <c r="E22" s="27"/>
       <c r="F22" s="27"/>
     </row>
@@ -12714,7 +12724,7 @@
       </c>
       <c r="J23" s="7">
         <f>COUNTIF(D23:D27,"NA")</f>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="24" ht="18.75" customHeight="1">
@@ -12753,7 +12763,9 @@
       <c r="C26" s="30" t="s">
         <v>89</v>
       </c>
-      <c r="D26" s="48"/>
+      <c r="D26" s="31" t="s">
+        <v>43</v>
+      </c>
       <c r="E26" s="30"/>
       <c r="F26" s="30"/>
     </row>
@@ -12765,7 +12777,9 @@
       <c r="C27" s="30" t="s">
         <v>90</v>
       </c>
-      <c r="D27" s="48"/>
+      <c r="D27" s="31" t="s">
+        <v>43</v>
+      </c>
       <c r="E27" s="30"/>
       <c r="F27" s="30"/>
     </row>
@@ -12777,7 +12791,7 @@
       <c r="C28" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="D28" s="49"/>
+      <c r="D28" s="48"/>
       <c r="E28" s="27"/>
       <c r="F28" s="27"/>
     </row>
@@ -12796,11 +12810,11 @@
       <c r="F29" s="30"/>
       <c r="G29" s="7">
         <f>COUNTIF(D29:D34,"Sim")</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H29" s="7">
         <f>COUNTIF(D29:D34,"Parcialmente")</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I29" s="7">
         <f>COUNTIF(D29:D34,"Não")</f>
@@ -12833,7 +12847,9 @@
       <c r="C31" s="30" t="s">
         <v>94</v>
       </c>
-      <c r="D31" s="48"/>
+      <c r="D31" s="31" t="s">
+        <v>72</v>
+      </c>
       <c r="E31" s="30"/>
       <c r="F31" s="30"/>
     </row>
@@ -12845,7 +12861,9 @@
       <c r="C32" s="30" t="s">
         <v>95</v>
       </c>
-      <c r="D32" s="48"/>
+      <c r="D32" s="31" t="s">
+        <v>46</v>
+      </c>
       <c r="E32" s="30"/>
       <c r="F32" s="30"/>
     </row>
@@ -12857,7 +12875,9 @@
       <c r="C33" s="30" t="s">
         <v>96</v>
       </c>
-      <c r="D33" s="48"/>
+      <c r="D33" s="31" t="s">
+        <v>46</v>
+      </c>
       <c r="E33" s="30"/>
       <c r="F33" s="30"/>
     </row>
@@ -12869,7 +12889,9 @@
       <c r="C34" s="30" t="s">
         <v>97</v>
       </c>
-      <c r="D34" s="48"/>
+      <c r="D34" s="31" t="s">
+        <v>46</v>
+      </c>
       <c r="E34" s="30"/>
       <c r="F34" s="30"/>
     </row>
@@ -12881,7 +12903,7 @@
       <c r="C35" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="D35" s="49"/>
+      <c r="D35" s="48"/>
       <c r="E35" s="27"/>
       <c r="F35" s="27"/>
     </row>
@@ -12893,16 +12915,18 @@
       <c r="C36" s="30" t="s">
         <v>69</v>
       </c>
-      <c r="D36" s="48"/>
+      <c r="D36" s="31" t="s">
+        <v>46</v>
+      </c>
       <c r="E36" s="30"/>
       <c r="F36" s="30"/>
       <c r="G36" s="7">
         <f>COUNTIF(D36:D38,"Sim")</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H36" s="7">
         <f>COUNTIF(D36:D38,"Parcialmente")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I36" s="7">
         <f>COUNTIF(D36:D38,"Não")</f>
@@ -12921,7 +12945,9 @@
       <c r="C37" s="30" t="s">
         <v>70</v>
       </c>
-      <c r="D37" s="48"/>
+      <c r="D37" s="31" t="s">
+        <v>46</v>
+      </c>
       <c r="E37" s="30"/>
       <c r="F37" s="30"/>
     </row>
@@ -12933,7 +12959,9 @@
       <c r="C38" s="30" t="s">
         <v>71</v>
       </c>
-      <c r="D38" s="48"/>
+      <c r="D38" s="31" t="s">
+        <v>72</v>
+      </c>
       <c r="E38" s="30"/>
       <c r="F38" s="30"/>
     </row>
@@ -12943,7 +12971,7 @@
       <c r="C39" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="D39" s="49"/>
+      <c r="D39" s="48"/>
       <c r="E39" s="27"/>
       <c r="F39" s="27"/>
     </row>
@@ -12955,7 +12983,9 @@
       <c r="C40" s="30" t="s">
         <v>98</v>
       </c>
-      <c r="D40" s="48"/>
+      <c r="D40" s="31" t="s">
+        <v>43</v>
+      </c>
       <c r="E40" s="30"/>
       <c r="F40" s="30"/>
       <c r="G40" s="7">
@@ -12972,7 +13002,7 @@
       </c>
       <c r="J40" s="7">
         <f>COUNTIF(D40:D41,"NA")</f>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="41" ht="18.75" customHeight="1">
@@ -12983,7 +13013,9 @@
       <c r="C41" s="30" t="s">
         <v>99</v>
       </c>
-      <c r="D41" s="48"/>
+      <c r="D41" s="31" t="s">
+        <v>43</v>
+      </c>
       <c r="E41" s="30"/>
       <c r="F41" s="30"/>
     </row>
@@ -16949,7 +16981,7 @@
       <c r="C6" s="30" t="s">
         <v>73</v>
       </c>
-      <c r="D6" s="48"/>
+      <c r="D6" s="49"/>
       <c r="E6" s="30"/>
       <c r="F6" s="30"/>
       <c r="G6" s="7">
@@ -16987,7 +17019,7 @@
       <c r="C8" s="30" t="s">
         <v>74</v>
       </c>
-      <c r="D8" s="48"/>
+      <c r="D8" s="49"/>
       <c r="E8" s="30"/>
       <c r="F8" s="30"/>
       <c r="G8" s="7">
@@ -17041,7 +17073,7 @@
       <c r="C10" s="30" t="s">
         <v>76</v>
       </c>
-      <c r="D10" s="48"/>
+      <c r="D10" s="49"/>
       <c r="E10" s="30"/>
       <c r="F10" s="30"/>
       <c r="G10" s="7">
@@ -17069,7 +17101,7 @@
       <c r="C11" s="30" t="s">
         <v>100</v>
       </c>
-      <c r="D11" s="48"/>
+      <c r="D11" s="49"/>
       <c r="E11" s="30"/>
       <c r="F11" s="30"/>
     </row>
@@ -17081,7 +17113,7 @@
       <c r="C12" s="30" t="s">
         <v>78</v>
       </c>
-      <c r="D12" s="48"/>
+      <c r="D12" s="49"/>
       <c r="E12" s="30"/>
       <c r="F12" s="30"/>
     </row>
@@ -17103,7 +17135,7 @@
       <c r="C14" s="30" t="s">
         <v>80</v>
       </c>
-      <c r="D14" s="48"/>
+      <c r="D14" s="49"/>
       <c r="E14" s="30"/>
       <c r="F14" s="30"/>
       <c r="G14" s="7">
@@ -17131,7 +17163,7 @@
       <c r="C15" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="D15" s="49"/>
+      <c r="D15" s="48"/>
       <c r="E15" s="27"/>
       <c r="F15" s="27"/>
     </row>
@@ -17143,7 +17175,7 @@
       <c r="C16" s="30" t="s">
         <v>101</v>
       </c>
-      <c r="D16" s="48"/>
+      <c r="D16" s="49"/>
       <c r="E16" s="30"/>
       <c r="F16" s="30"/>
       <c r="G16" s="7">
@@ -17171,7 +17203,7 @@
       <c r="C17" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="D17" s="49"/>
+      <c r="D17" s="48"/>
       <c r="E17" s="27"/>
       <c r="F17" s="27"/>
     </row>
@@ -17183,7 +17215,7 @@
       <c r="C18" s="30" t="s">
         <v>102</v>
       </c>
-      <c r="D18" s="48"/>
+      <c r="D18" s="49"/>
       <c r="E18" s="30"/>
       <c r="F18" s="30"/>
       <c r="G18" s="7">
@@ -17211,7 +17243,7 @@
       <c r="C19" s="30" t="s">
         <v>87</v>
       </c>
-      <c r="D19" s="48"/>
+      <c r="D19" s="49"/>
       <c r="E19" s="30"/>
       <c r="F19" s="30"/>
     </row>
@@ -17223,7 +17255,7 @@
       <c r="C20" s="30" t="s">
         <v>88</v>
       </c>
-      <c r="D20" s="48"/>
+      <c r="D20" s="49"/>
       <c r="E20" s="30"/>
       <c r="F20" s="30"/>
     </row>
@@ -17235,7 +17267,7 @@
       <c r="C21" s="30" t="s">
         <v>89</v>
       </c>
-      <c r="D21" s="48"/>
+      <c r="D21" s="49"/>
       <c r="E21" s="30"/>
       <c r="F21" s="30"/>
     </row>
@@ -17247,7 +17279,7 @@
       <c r="C22" s="30" t="s">
         <v>90</v>
       </c>
-      <c r="D22" s="48"/>
+      <c r="D22" s="49"/>
       <c r="E22" s="30"/>
       <c r="F22" s="30"/>
     </row>
@@ -17259,7 +17291,7 @@
       <c r="C23" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="D23" s="49"/>
+      <c r="D23" s="48"/>
       <c r="E23" s="27"/>
       <c r="F23" s="27"/>
     </row>
@@ -17271,7 +17303,7 @@
       <c r="C24" s="34" t="s">
         <v>45</v>
       </c>
-      <c r="D24" s="48"/>
+      <c r="D24" s="49"/>
       <c r="E24" s="30"/>
       <c r="F24" s="30"/>
       <c r="G24" s="7">
@@ -17299,7 +17331,7 @@
       <c r="C25" s="30" t="s">
         <v>104</v>
       </c>
-      <c r="D25" s="48"/>
+      <c r="D25" s="49"/>
       <c r="E25" s="30"/>
       <c r="F25" s="30"/>
     </row>
@@ -17311,7 +17343,7 @@
       <c r="C26" s="30" t="s">
         <v>105</v>
       </c>
-      <c r="D26" s="48"/>
+      <c r="D26" s="49"/>
       <c r="E26" s="30"/>
       <c r="F26" s="30"/>
     </row>
@@ -17323,7 +17355,7 @@
       <c r="C27" s="30" t="s">
         <v>106</v>
       </c>
-      <c r="D27" s="48"/>
+      <c r="D27" s="49"/>
       <c r="E27" s="30"/>
       <c r="F27" s="30"/>
     </row>
@@ -17335,7 +17367,7 @@
       <c r="C28" s="30" t="s">
         <v>107</v>
       </c>
-      <c r="D28" s="48"/>
+      <c r="D28" s="49"/>
       <c r="E28" s="30"/>
       <c r="F28" s="30"/>
     </row>
@@ -17347,7 +17379,7 @@
       <c r="C29" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="D29" s="49"/>
+      <c r="D29" s="48"/>
       <c r="E29" s="27"/>
       <c r="F29" s="27"/>
     </row>
@@ -17359,7 +17391,7 @@
       <c r="C30" s="30" t="s">
         <v>92</v>
       </c>
-      <c r="D30" s="48"/>
+      <c r="D30" s="49"/>
       <c r="E30" s="30"/>
       <c r="F30" s="30"/>
       <c r="G30" s="7">
@@ -17387,7 +17419,7 @@
       <c r="C31" s="30" t="s">
         <v>108</v>
       </c>
-      <c r="D31" s="48"/>
+      <c r="D31" s="49"/>
       <c r="E31" s="30"/>
       <c r="F31" s="30"/>
     </row>
@@ -17399,7 +17431,7 @@
       <c r="C32" s="30" t="s">
         <v>109</v>
       </c>
-      <c r="D32" s="48"/>
+      <c r="D32" s="49"/>
       <c r="E32" s="30"/>
       <c r="F32" s="30"/>
     </row>
@@ -17411,7 +17443,7 @@
       <c r="C33" s="30" t="s">
         <v>96</v>
       </c>
-      <c r="D33" s="48"/>
+      <c r="D33" s="49"/>
       <c r="E33" s="30"/>
       <c r="F33" s="30"/>
     </row>
@@ -17423,7 +17455,7 @@
       <c r="C34" s="30" t="s">
         <v>97</v>
       </c>
-      <c r="D34" s="48"/>
+      <c r="D34" s="49"/>
       <c r="E34" s="30"/>
       <c r="F34" s="30"/>
     </row>
@@ -17435,7 +17467,7 @@
       <c r="C35" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="D35" s="49"/>
+      <c r="D35" s="48"/>
       <c r="E35" s="27"/>
       <c r="F35" s="27"/>
     </row>
@@ -17447,7 +17479,7 @@
       <c r="C36" s="30" t="s">
         <v>69</v>
       </c>
-      <c r="D36" s="48"/>
+      <c r="D36" s="49"/>
       <c r="E36" s="30"/>
       <c r="F36" s="30"/>
       <c r="G36" s="7">
@@ -17475,7 +17507,7 @@
       <c r="C37" s="30" t="s">
         <v>70</v>
       </c>
-      <c r="D37" s="48"/>
+      <c r="D37" s="49"/>
       <c r="E37" s="30"/>
       <c r="F37" s="30"/>
     </row>
@@ -17487,7 +17519,7 @@
       <c r="C38" s="30" t="s">
         <v>71</v>
       </c>
-      <c r="D38" s="48"/>
+      <c r="D38" s="49"/>
       <c r="E38" s="30"/>
       <c r="F38" s="30"/>
     </row>
@@ -17497,7 +17529,7 @@
       <c r="C39" s="30" t="s">
         <v>110</v>
       </c>
-      <c r="D39" s="48"/>
+      <c r="D39" s="49"/>
       <c r="E39" s="30"/>
       <c r="F39" s="30"/>
     </row>
@@ -17507,7 +17539,7 @@
       <c r="C40" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="D40" s="49"/>
+      <c r="D40" s="48"/>
       <c r="E40" s="27"/>
       <c r="F40" s="27"/>
     </row>
@@ -17519,7 +17551,7 @@
       <c r="C41" s="30" t="s">
         <v>98</v>
       </c>
-      <c r="D41" s="48"/>
+      <c r="D41" s="49"/>
       <c r="E41" s="30"/>
       <c r="F41" s="30"/>
       <c r="G41" s="7">
@@ -17547,7 +17579,7 @@
       <c r="C42" s="30" t="s">
         <v>99</v>
       </c>
-      <c r="D42" s="48"/>
+      <c r="D42" s="49"/>
       <c r="E42" s="30"/>
       <c r="F42" s="30"/>
     </row>
@@ -21489,7 +21521,7 @@
       <c r="C6" s="30" t="s">
         <v>73</v>
       </c>
-      <c r="D6" s="48"/>
+      <c r="D6" s="49"/>
       <c r="E6" s="30"/>
       <c r="F6" s="30"/>
       <c r="G6" s="7">
@@ -21527,7 +21559,7 @@
       <c r="C8" s="30" t="s">
         <v>74</v>
       </c>
-      <c r="D8" s="48"/>
+      <c r="D8" s="49"/>
       <c r="E8" s="30"/>
       <c r="F8" s="30"/>
       <c r="G8" s="7">
@@ -21581,7 +21613,7 @@
       <c r="C10" s="30" t="s">
         <v>76</v>
       </c>
-      <c r="D10" s="48"/>
+      <c r="D10" s="49"/>
       <c r="E10" s="30"/>
       <c r="F10" s="30"/>
       <c r="G10" s="7">
@@ -21609,7 +21641,7 @@
       <c r="C11" s="30" t="s">
         <v>100</v>
       </c>
-      <c r="D11" s="48"/>
+      <c r="D11" s="49"/>
       <c r="E11" s="30"/>
       <c r="F11" s="30"/>
     </row>
@@ -21621,7 +21653,7 @@
       <c r="C12" s="30" t="s">
         <v>78</v>
       </c>
-      <c r="D12" s="48"/>
+      <c r="D12" s="49"/>
       <c r="E12" s="30"/>
       <c r="F12" s="30"/>
     </row>
@@ -21643,7 +21675,7 @@
       <c r="C14" s="30" t="s">
         <v>80</v>
       </c>
-      <c r="D14" s="48"/>
+      <c r="D14" s="49"/>
       <c r="E14" s="30"/>
       <c r="F14" s="30"/>
       <c r="G14" s="7">
@@ -21671,7 +21703,7 @@
       <c r="C15" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="D15" s="49"/>
+      <c r="D15" s="48"/>
       <c r="E15" s="27"/>
       <c r="F15" s="27"/>
     </row>
@@ -21683,7 +21715,7 @@
       <c r="C16" s="30" t="s">
         <v>101</v>
       </c>
-      <c r="D16" s="48"/>
+      <c r="D16" s="49"/>
       <c r="E16" s="30"/>
       <c r="F16" s="30"/>
       <c r="G16" s="7">
@@ -21711,7 +21743,7 @@
       <c r="C17" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="D17" s="49"/>
+      <c r="D17" s="48"/>
       <c r="E17" s="27"/>
       <c r="F17" s="27"/>
     </row>
@@ -21723,7 +21755,7 @@
       <c r="C18" s="30" t="s">
         <v>111</v>
       </c>
-      <c r="D18" s="48"/>
+      <c r="D18" s="49"/>
       <c r="E18" s="30"/>
       <c r="F18" s="30"/>
       <c r="G18" s="7">
@@ -21751,7 +21783,7 @@
       <c r="C19" s="30" t="s">
         <v>112</v>
       </c>
-      <c r="D19" s="48"/>
+      <c r="D19" s="49"/>
       <c r="E19" s="30"/>
       <c r="F19" s="30"/>
     </row>
@@ -21763,7 +21795,7 @@
       <c r="C20" s="30" t="s">
         <v>88</v>
       </c>
-      <c r="D20" s="48"/>
+      <c r="D20" s="49"/>
       <c r="E20" s="30"/>
       <c r="F20" s="30"/>
     </row>
@@ -21775,7 +21807,7 @@
       <c r="C21" s="30" t="s">
         <v>113</v>
       </c>
-      <c r="D21" s="48"/>
+      <c r="D21" s="49"/>
       <c r="E21" s="30"/>
       <c r="F21" s="30"/>
     </row>
@@ -21787,7 +21819,7 @@
       <c r="C22" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="D22" s="49"/>
+      <c r="D22" s="48"/>
       <c r="E22" s="27"/>
       <c r="F22" s="27"/>
     </row>
@@ -21799,7 +21831,7 @@
       <c r="C23" s="30" t="s">
         <v>114</v>
       </c>
-      <c r="D23" s="48"/>
+      <c r="D23" s="49"/>
       <c r="E23" s="30"/>
       <c r="F23" s="30"/>
       <c r="G23" s="7">
@@ -21827,7 +21859,7 @@
       <c r="C24" s="30" t="s">
         <v>107</v>
       </c>
-      <c r="D24" s="48"/>
+      <c r="D24" s="49"/>
       <c r="E24" s="30"/>
       <c r="F24" s="30"/>
     </row>
@@ -21839,7 +21871,7 @@
       <c r="C25" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="D25" s="49"/>
+      <c r="D25" s="48"/>
       <c r="E25" s="27"/>
       <c r="F25" s="27"/>
       <c r="G25" s="35"/>
@@ -21871,7 +21903,7 @@
       <c r="C26" s="34" t="s">
         <v>45</v>
       </c>
-      <c r="D26" s="48"/>
+      <c r="D26" s="49"/>
       <c r="E26" s="30"/>
       <c r="F26" s="30"/>
       <c r="G26" s="7">
@@ -21915,7 +21947,7 @@
       <c r="C27" s="30" t="s">
         <v>116</v>
       </c>
-      <c r="D27" s="48"/>
+      <c r="D27" s="49"/>
       <c r="E27" s="30"/>
       <c r="F27" s="30"/>
       <c r="G27" s="35"/>
@@ -21945,7 +21977,7 @@
       <c r="C28" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="D28" s="49"/>
+      <c r="D28" s="48"/>
       <c r="E28" s="27"/>
       <c r="F28" s="27"/>
     </row>
@@ -21957,7 +21989,7 @@
       <c r="C29" s="34" t="s">
         <v>45</v>
       </c>
-      <c r="D29" s="48"/>
+      <c r="D29" s="49"/>
       <c r="E29" s="30"/>
       <c r="F29" s="30"/>
       <c r="G29" s="7">
@@ -21985,7 +22017,7 @@
       <c r="C30" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="D30" s="49"/>
+      <c r="D30" s="48"/>
       <c r="E30" s="27"/>
       <c r="F30" s="27"/>
     </row>
@@ -21997,7 +22029,7 @@
       <c r="C31" s="30" t="s">
         <v>92</v>
       </c>
-      <c r="D31" s="48"/>
+      <c r="D31" s="49"/>
       <c r="E31" s="30"/>
       <c r="F31" s="30"/>
       <c r="G31" s="7">
@@ -22025,7 +22057,7 @@
       <c r="C32" s="30" t="s">
         <v>108</v>
       </c>
-      <c r="D32" s="48"/>
+      <c r="D32" s="49"/>
       <c r="E32" s="30"/>
       <c r="F32" s="30"/>
     </row>
@@ -22037,7 +22069,7 @@
       <c r="C33" s="30" t="s">
         <v>109</v>
       </c>
-      <c r="D33" s="48"/>
+      <c r="D33" s="49"/>
       <c r="E33" s="30"/>
       <c r="F33" s="30"/>
     </row>
@@ -22049,7 +22081,7 @@
       <c r="C34" s="30" t="s">
         <v>117</v>
       </c>
-      <c r="D34" s="48"/>
+      <c r="D34" s="49"/>
       <c r="E34" s="30"/>
       <c r="F34" s="30"/>
     </row>
@@ -22061,7 +22093,7 @@
       <c r="C35" s="30" t="s">
         <v>97</v>
       </c>
-      <c r="D35" s="48"/>
+      <c r="D35" s="49"/>
       <c r="E35" s="30"/>
       <c r="F35" s="30"/>
     </row>
@@ -22073,7 +22105,7 @@
       <c r="C36" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="D36" s="49"/>
+      <c r="D36" s="48"/>
       <c r="E36" s="27"/>
       <c r="F36" s="27"/>
     </row>
@@ -22085,7 +22117,7 @@
       <c r="C37" s="30" t="s">
         <v>69</v>
       </c>
-      <c r="D37" s="48"/>
+      <c r="D37" s="49"/>
       <c r="E37" s="30"/>
       <c r="F37" s="30"/>
       <c r="G37" s="7">
@@ -22113,7 +22145,7 @@
       <c r="C38" s="30" t="s">
         <v>70</v>
       </c>
-      <c r="D38" s="48"/>
+      <c r="D38" s="49"/>
       <c r="E38" s="30"/>
       <c r="F38" s="30"/>
     </row>
@@ -22125,7 +22157,7 @@
       <c r="C39" s="30" t="s">
         <v>71</v>
       </c>
-      <c r="D39" s="48"/>
+      <c r="D39" s="49"/>
       <c r="E39" s="30"/>
       <c r="F39" s="30"/>
     </row>
@@ -22135,7 +22167,7 @@
       <c r="C40" s="30" t="s">
         <v>110</v>
       </c>
-      <c r="D40" s="48"/>
+      <c r="D40" s="49"/>
       <c r="E40" s="30"/>
       <c r="F40" s="30"/>
     </row>
@@ -22145,7 +22177,7 @@
       <c r="C41" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="D41" s="49"/>
+      <c r="D41" s="48"/>
       <c r="E41" s="27"/>
       <c r="F41" s="27"/>
     </row>
@@ -22157,7 +22189,7 @@
       <c r="C42" s="30" t="s">
         <v>98</v>
       </c>
-      <c r="D42" s="48"/>
+      <c r="D42" s="49"/>
       <c r="E42" s="30"/>
       <c r="F42" s="30"/>
       <c r="G42" s="7">
@@ -22185,7 +22217,7 @@
       <c r="C43" s="30" t="s">
         <v>99</v>
       </c>
-      <c r="D43" s="48"/>
+      <c r="D43" s="49"/>
       <c r="E43" s="30"/>
       <c r="F43" s="30"/>
     </row>

</xml_diff>

<commit_message>
Adição Guia de Implantação
</commit_message>
<xml_diff>
--- a/SGB/6.Gerenciamento de Projeto/SGB - Checklist Verificacao de Projeto.xlsx
+++ b/SGB/6.Gerenciamento de Projeto/SGB - Checklist Verificacao de Projeto.xlsx
@@ -241,7 +241,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="118">
   <si>
     <t>IAP - Indicador de Aderência ao Processo (70% a 100%)</t>
   </si>
@@ -1072,11 +1072,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="1275024991"/>
-        <c:axId val="1505917724"/>
+        <c:axId val="1048153949"/>
+        <c:axId val="1111896403"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1275024991"/>
+        <c:axId val="1048153949"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1128,10 +1128,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1505917724"/>
+        <c:crossAx val="1111896403"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1505917724"/>
+        <c:axId val="1111896403"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1195,7 +1195,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1275024991"/>
+        <c:crossAx val="1048153949"/>
       </c:valAx>
     </c:plotArea>
     <c:plotVisOnly val="1"/>
@@ -1350,11 +1350,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="1020871828"/>
-        <c:axId val="111446715"/>
+        <c:axId val="459828231"/>
+        <c:axId val="1983046349"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1020871828"/>
+        <c:axId val="459828231"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1406,10 +1406,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="111446715"/>
+        <c:crossAx val="1983046349"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="111446715"/>
+        <c:axId val="1983046349"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1473,7 +1473,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1020871828"/>
+        <c:crossAx val="459828231"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -1646,11 +1646,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="1764164371"/>
-        <c:axId val="1856139130"/>
+        <c:axId val="2061196936"/>
+        <c:axId val="203813717"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1764164371"/>
+        <c:axId val="2061196936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1702,10 +1702,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1856139130"/>
+        <c:crossAx val="203813717"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1856139130"/>
+        <c:axId val="203813717"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1769,7 +1769,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1764164371"/>
+        <c:crossAx val="2061196936"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -1838,6 +1838,16 @@
               <c:f>Detalhado!$B$22</c:f>
             </c:strRef>
           </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
           <c:cat>
             <c:strRef>
               <c:f>Detalhado!$A$23:$A$34</c:f>
@@ -1858,6 +1868,16 @@
               <c:f>Detalhado!$C$22</c:f>
             </c:strRef>
           </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
           <c:cat>
             <c:strRef>
               <c:f>Detalhado!$A$23:$A$34</c:f>
@@ -1878,6 +1898,16 @@
               <c:f>Detalhado!$D$22</c:f>
             </c:strRef>
           </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
           <c:cat>
             <c:strRef>
               <c:f>Detalhado!$A$23:$A$34</c:f>
@@ -1898,6 +1928,16 @@
               <c:f>Detalhado!$E$22</c:f>
             </c:strRef>
           </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
           <c:cat>
             <c:strRef>
               <c:f>Detalhado!$A$23:$A$34</c:f>
@@ -1910,11 +1950,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="1620240080"/>
-        <c:axId val="257231042"/>
+        <c:axId val="1684654413"/>
+        <c:axId val="1731146075"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1620240080"/>
+        <c:axId val="1684654413"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1966,22 +2006,65 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="257231042"/>
+        <c:crossAx val="1731146075"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="257231042"/>
+        <c:axId val="1731146075"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:rPr>
+                  <a:t/>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
+          <a:ln/>
         </c:spPr>
-        <c:crossAx val="1620240080"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1684654413"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -2122,11 +2205,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="669068495"/>
-        <c:axId val="194778608"/>
+        <c:axId val="1285628610"/>
+        <c:axId val="1816488216"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="669068495"/>
+        <c:axId val="1285628610"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2178,10 +2261,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="194778608"/>
+        <c:crossAx val="1816488216"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="194778608"/>
+        <c:axId val="1816488216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2193,7 +2276,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="669068495"/>
+        <c:crossAx val="1285628610"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -2608,7 +2691,7 @@
       </c>
       <c r="B4" s="5">
         <f>'Ver-Elaboração1'!$F$2</f>
-        <v>0.8636363636</v>
+        <v>0.8181818182</v>
       </c>
     </row>
     <row r="5">
@@ -4339,11 +4422,11 @@
       </c>
       <c r="O7" s="8">
         <f>('Ver-Elaboração1'!$G$18/SUM('Ver-Elaboração1'!$G$18:'Ver-Elaboração1'!$J$18))</f>
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="P7" s="8">
         <f>('Ver-Elaboração1'!$H$18/SUM('Ver-Elaboração1'!$G$18:'Ver-Elaboração1'!$J$18))</f>
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="Q7" s="8">
         <f>('Ver-Elaboração1'!$I$18/SUM('Ver-Elaboração1'!$G$18:'Ver-Elaboração1'!$J$18))</f>
@@ -4459,11 +4542,11 @@
       </c>
       <c r="O10" s="8">
         <f>('Ver-Elaboração1'!$G$29/SUM('Ver-Elaboração1'!$G$29:'Ver-Elaboração1'!$J$29))</f>
-        <v>1</v>
+        <v>0.6666666667</v>
       </c>
       <c r="P10" s="8">
         <f>('Ver-Elaboração1'!$H$29/SUM('Ver-Elaboração1'!$G$29:'Ver-Elaboração1'!$J$29))</f>
-        <v>0</v>
+        <v>0.3333333333</v>
       </c>
       <c r="Q10" s="8">
         <f>('Ver-Elaboração1'!$I$29/SUM('Ver-Elaboração1'!$G$29:'Ver-Elaboração1'!$J$29))</f>
@@ -4673,21 +4756,21 @@
       <c r="A26" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B26" s="9" t="str">
+      <c r="B26" s="9">
         <f>('Ver-Construção1'!$G$14/SUM('Ver-Construção1'!$G$14:'Ver-Construção1'!$J$14))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C26" s="9" t="str">
+        <v>0</v>
+      </c>
+      <c r="C26" s="9">
         <f>('Ver-Construção1'!$H$14/SUM('Ver-Construção1'!$G$14:'Ver-Construção1'!$J$14))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D26" s="9" t="str">
+        <v>0</v>
+      </c>
+      <c r="D26" s="9">
         <f>('Ver-Construção1'!$I$14/SUM('Ver-Construção1'!$G$14:'Ver-Construção1'!$J$14))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E26" s="9" t="str">
+        <v>0</v>
+      </c>
+      <c r="E26" s="9">
         <f>('Ver-Construção1'!$J$14/SUM('Ver-Construção1'!$G$14:'Ver-Construção1'!$J$14))</f>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
       <c r="M26" s="7" t="s">
         <v>14</v>
@@ -8492,7 +8575,7 @@
       <c r="E2" s="15"/>
       <c r="F2" s="16">
         <f>COUNTIF(D5:D41,"Sim")/(COUNTA(D5:D42)-COUNTIF(D5:D42,"NA"))</f>
-        <v>0.8636363636</v>
+        <v>0.8181818182</v>
       </c>
     </row>
     <row r="3" ht="18.75" customHeight="1">
@@ -8804,11 +8887,11 @@
       <c r="F18" s="30"/>
       <c r="G18" s="7">
         <f>COUNTIF(D18:D21,"Sim")</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H18" s="7">
         <f>COUNTIF(D18:D21,"Parcialmente")</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I18" s="7">
         <f>COUNTIF(D18:D21,"Não")</f>
@@ -8827,8 +8910,8 @@
       <c r="C19" s="34" t="s">
         <v>83</v>
       </c>
-      <c r="D19" s="31" t="s">
-        <v>72</v>
+      <c r="D19" s="45" t="s">
+        <v>46</v>
       </c>
       <c r="E19" s="30"/>
       <c r="F19" s="30"/>
@@ -8841,7 +8924,7 @@
       <c r="C20" s="30" t="s">
         <v>84</v>
       </c>
-      <c r="D20" s="31" t="s">
+      <c r="D20" s="45" t="s">
         <v>72</v>
       </c>
       <c r="E20" s="30"/>
@@ -8931,7 +9014,7 @@
       <c r="C24" s="30" t="s">
         <v>87</v>
       </c>
-      <c r="D24" s="31" t="s">
+      <c r="D24" s="45" t="s">
         <v>46</v>
       </c>
       <c r="E24" s="30"/>
@@ -8945,7 +9028,7 @@
       <c r="C25" s="30" t="s">
         <v>88</v>
       </c>
-      <c r="D25" s="31" t="s">
+      <c r="D25" s="45" t="s">
         <v>46</v>
       </c>
       <c r="E25" s="30"/>
@@ -9006,11 +9089,11 @@
       <c r="F29" s="30"/>
       <c r="G29" s="7">
         <f>COUNTIF(D29:D34,"Sim")</f>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="H29" s="7">
         <f>COUNTIF(D29:D34,"Parcialmente")</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I29" s="7">
         <f>COUNTIF(D29:D34,"Não")</f>
@@ -9030,7 +9113,7 @@
         <v>93</v>
       </c>
       <c r="D30" s="45" t="s">
-        <v>46</v>
+        <v>72</v>
       </c>
       <c r="E30" s="30"/>
       <c r="F30" s="30"/>
@@ -9044,7 +9127,7 @@
         <v>94</v>
       </c>
       <c r="D31" s="45" t="s">
-        <v>46</v>
+        <v>72</v>
       </c>
       <c r="E31" s="30"/>
       <c r="F31" s="30"/>
@@ -9141,7 +9224,7 @@
       <c r="C37" s="30" t="s">
         <v>70</v>
       </c>
-      <c r="D37" s="31" t="s">
+      <c r="D37" s="45" t="s">
         <v>46</v>
       </c>
       <c r="E37" s="30"/>
@@ -11054,7 +11137,9 @@
       <c r="C14" s="30" t="s">
         <v>80</v>
       </c>
-      <c r="D14" s="31"/>
+      <c r="D14" s="45" t="s">
+        <v>43</v>
+      </c>
       <c r="E14" s="30"/>
       <c r="F14" s="30"/>
       <c r="G14" s="7">
@@ -11071,7 +11156,7 @@
       </c>
       <c r="J14" s="7">
         <f>COUNTIF(D14,"NA")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" ht="15.0" customHeight="1">

</xml_diff>

<commit_message>
Realização do Checklist da fase de construção, alteração do planejamento para implantação na nuvem
</commit_message>
<xml_diff>
--- a/SGB/6.Gerenciamento de Projeto/SGB - Checklist Verificacao de Projeto.xlsx
+++ b/SGB/6.Gerenciamento de Projeto/SGB - Checklist Verificacao de Projeto.xlsx
@@ -241,7 +241,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="118">
   <si>
     <t>IAP - Indicador de Aderência ao Processo (70% a 100%)</t>
   </si>
@@ -1072,11 +1072,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="1048153949"/>
-        <c:axId val="1111896403"/>
+        <c:axId val="1277942220"/>
+        <c:axId val="765381546"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1048153949"/>
+        <c:axId val="1277942220"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1128,10 +1128,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1111896403"/>
+        <c:crossAx val="765381546"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1111896403"/>
+        <c:axId val="765381546"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1195,7 +1195,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1048153949"/>
+        <c:crossAx val="1277942220"/>
       </c:valAx>
     </c:plotArea>
     <c:plotVisOnly val="1"/>
@@ -1350,11 +1350,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="459828231"/>
-        <c:axId val="1983046349"/>
+        <c:axId val="8186131"/>
+        <c:axId val="820519570"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="459828231"/>
+        <c:axId val="8186131"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1406,10 +1406,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1983046349"/>
+        <c:crossAx val="820519570"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1983046349"/>
+        <c:axId val="820519570"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1473,7 +1473,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="459828231"/>
+        <c:crossAx val="8186131"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -1646,11 +1646,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="2061196936"/>
-        <c:axId val="203813717"/>
+        <c:axId val="934834915"/>
+        <c:axId val="297186432"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2061196936"/>
+        <c:axId val="934834915"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1702,10 +1702,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="203813717"/>
+        <c:crossAx val="297186432"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="203813717"/>
+        <c:axId val="297186432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1769,7 +1769,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2061196936"/>
+        <c:crossAx val="934834915"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -1950,11 +1950,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="1684654413"/>
-        <c:axId val="1731146075"/>
+        <c:axId val="736625280"/>
+        <c:axId val="515221719"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1684654413"/>
+        <c:axId val="736625280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2006,10 +2006,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1731146075"/>
+        <c:crossAx val="515221719"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1731146075"/>
+        <c:axId val="515221719"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2064,7 +2064,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1684654413"/>
+        <c:crossAx val="736625280"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -2205,11 +2205,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="1285628610"/>
-        <c:axId val="1816488216"/>
+        <c:axId val="2096883095"/>
+        <c:axId val="665270780"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1285628610"/>
+        <c:axId val="2096883095"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2261,10 +2261,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1816488216"/>
+        <c:crossAx val="665270780"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1816488216"/>
+        <c:axId val="665270780"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2276,7 +2276,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="1285628610"/>
+        <c:crossAx val="2096883095"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -2691,16 +2691,16 @@
       </c>
       <c r="B4" s="5">
         <f>'Ver-Elaboração1'!$F$2</f>
-        <v>0.8181818182</v>
+        <v>0.8636363636</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="5" t="str">
+      <c r="B5" s="5">
         <f>'Ver-Construção1'!$F$2</f>
-        <v>#DIV/0!</v>
+        <v>0.8695652174</v>
       </c>
     </row>
     <row r="6">
@@ -4542,11 +4542,11 @@
       </c>
       <c r="O10" s="8">
         <f>('Ver-Elaboração1'!$G$29/SUM('Ver-Elaboração1'!$G$29:'Ver-Elaboração1'!$J$29))</f>
-        <v>0.6666666667</v>
+        <v>0.8333333333</v>
       </c>
       <c r="P10" s="8">
         <f>('Ver-Elaboração1'!$H$29/SUM('Ver-Elaboração1'!$G$29:'Ver-Elaboração1'!$J$29))</f>
-        <v>0.3333333333</v>
+        <v>0.1666666667</v>
       </c>
       <c r="Q10" s="8">
         <f>('Ver-Elaboração1'!$I$29/SUM('Ver-Elaboração1'!$G$29:'Ver-Elaboração1'!$J$29))</f>
@@ -4659,42 +4659,42 @@
       <c r="A23" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B23" s="8" t="str">
+      <c r="B23" s="8">
         <f>('Ver-Construção1'!$G$6/SUM('Ver-Construção1'!$G$6:'Ver-Construção1'!$J$6))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C23" s="9" t="str">
+        <v>1</v>
+      </c>
+      <c r="C23" s="9">
         <f>('Ver-Construção1'!$H$6/SUM('Ver-Construção1'!$G$6:'Ver-Construção1'!$J$6))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D23" s="9" t="str">
+        <v>0</v>
+      </c>
+      <c r="D23" s="9">
         <f>('Ver-Construção1'!$I$6/SUM('Ver-Construção1'!$G$6:'Ver-Construção1'!$J$6))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E23" s="9" t="str">
+        <v>0</v>
+      </c>
+      <c r="E23" s="9">
         <f>('Ver-Construção1'!$J$6/SUM('Ver-Construção1'!$G$6:'Ver-Construção1'!$J$6))</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" ht="15.75" customHeight="1">
       <c r="A24" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B24" s="8" t="str">
+      <c r="B24" s="8">
         <f>('Ver-Construção1'!$G$8/SUM('Ver-Construção1'!$G$8:'Ver-Construção1'!$J$8))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C24" s="9" t="str">
+        <v>1</v>
+      </c>
+      <c r="C24" s="9">
         <f>('Ver-Construção1'!$H$8/SUM('Ver-Construção1'!$G$8:'Ver-Construção1'!$J$8))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D24" s="9" t="str">
+        <v>0</v>
+      </c>
+      <c r="D24" s="9">
         <f>('Ver-Construção1'!$I$8/SUM('Ver-Construção1'!$G$8:'Ver-Construção1'!$J$8))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E24" s="9" t="str">
+        <v>0</v>
+      </c>
+      <c r="E24" s="9">
         <f>('Ver-Construção1'!$J$8/SUM('Ver-Construção1'!$G$8:'Ver-Construção1'!$J$8))</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="M24" s="7" t="s">
         <v>7</v>
@@ -4716,21 +4716,21 @@
       <c r="A25" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B25" s="8" t="str">
+      <c r="B25" s="8">
         <f>('Ver-Construção1'!$G$10/SUM('Ver-Construção1'!$G$10:'Ver-Construção1'!$J$10))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C25" s="9" t="str">
+        <v>1</v>
+      </c>
+      <c r="C25" s="9">
         <f>('Ver-Construção1'!$G$10/SUM('Ver-Construção1'!$G$10:'Ver-Construção1'!$J$10))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D25" s="9" t="str">
+        <v>1</v>
+      </c>
+      <c r="D25" s="9">
         <f>('Ver-Construção1'!$I$10/SUM('Ver-Construção1'!$G$10:'Ver-Construção1'!$J$10))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E25" s="9" t="str">
+        <v>0</v>
+      </c>
+      <c r="E25" s="9">
         <f>('Ver-Construção1'!$J$10/SUM('Ver-Construção1'!$G$10:'Ver-Construção1'!$J$10))</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="M25" s="7" t="s">
         <v>13</v>
@@ -4836,21 +4836,21 @@
       <c r="A28" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B28" s="9" t="str">
+      <c r="B28" s="9">
         <f>('Ver-Construção1'!$G$16/SUM('Ver-Construção1'!$G$16:'Ver-Construção1'!$J$16))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C28" s="9" t="str">
+        <v>1</v>
+      </c>
+      <c r="C28" s="9">
         <f>('Ver-Construção1'!$H$16/SUM('Ver-Construção1'!$G$16:'Ver-Construção1'!$J$16))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D28" s="9" t="str">
+        <v>0</v>
+      </c>
+      <c r="D28" s="9">
         <f>('Ver-Construção1'!$I$16/SUM('Ver-Construção1'!$G$16:'Ver-Construção1'!$J$16))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E28" s="9" t="str">
+        <v>0</v>
+      </c>
+      <c r="E28" s="9">
         <f>('Ver-Construção1'!$J$16/SUM('Ver-Construção1'!$G$16:'Ver-Construção1'!$J$16))</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="M28" s="7" t="s">
         <v>16</v>
@@ -4916,21 +4916,21 @@
       <c r="A30" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="B30" s="9" t="str">
+      <c r="B30" s="9">
         <f>('Ver-Construção1'!$G$18/SUM('Ver-Construção1'!$G$18:'Ver-Construção1'!$J$18))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C30" s="9" t="str">
+        <v>0.6</v>
+      </c>
+      <c r="C30" s="9">
         <f>('Ver-Construção1'!$H$18/SUM('Ver-Construção1'!$G$18:'Ver-Construção1'!$J$18))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D30" s="9" t="str">
+        <v>0.4</v>
+      </c>
+      <c r="D30" s="9">
         <f>('Ver-Construção1'!$I$18/SUM('Ver-Construção1'!$G$18:'Ver-Construção1'!$J$18))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E30" s="9" t="str">
+        <v>0</v>
+      </c>
+      <c r="E30" s="9">
         <f>('Ver-Construção1'!$J$18/SUM('Ver-Construção1'!$G$18:'Ver-Construção1'!$J$18))</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="M30" s="7" t="s">
         <v>18</v>
@@ -4956,21 +4956,21 @@
       <c r="A31" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="B31" s="9" t="str">
+      <c r="B31" s="9">
         <f>('Ver-Construção1'!$G$24/SUM('Ver-Construção1'!$G$24:'Ver-Construção1'!$J$24))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C31" s="9" t="str">
+        <v>1</v>
+      </c>
+      <c r="C31" s="9">
         <f>('Ver-Construção1'!$H$24/SUM('Ver-Construção1'!$G$24:'Ver-Construção1'!$J$24))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D31" s="9" t="str">
+        <v>0</v>
+      </c>
+      <c r="D31" s="9">
         <f>('Ver-Construção1'!$I$24/SUM('Ver-Construção1'!$G$24:'Ver-Construção1'!$J$24))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E31" s="9" t="str">
+        <v>0</v>
+      </c>
+      <c r="E31" s="9">
         <f>('Ver-Construção1'!$J$24/SUM('Ver-Construção1'!$G$24:'Ver-Construção1'!$J$24))</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="M31" s="7" t="s">
         <v>22</v>
@@ -4996,21 +4996,21 @@
       <c r="A32" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="B32" s="9" t="str">
+      <c r="B32" s="9">
         <f>('Ver-Construção1'!$G$30/SUM('Ver-Construção1'!$G$30:'Ver-Construção1'!$J$30))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C32" s="9" t="str">
+        <v>0.6</v>
+      </c>
+      <c r="C32" s="9">
         <f>('Ver-Construção1'!$H$30/SUM('Ver-Construção1'!$G$30:'Ver-Construção1'!$J$30))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D32" s="9" t="str">
+        <v>0</v>
+      </c>
+      <c r="D32" s="9">
         <f>('Ver-Construção1'!$I$30/SUM('Ver-Construção1'!$G$30:'Ver-Construção1'!$J$30))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E32" s="9" t="str">
+        <v>0</v>
+      </c>
+      <c r="E32" s="9">
         <f>('Ver-Construção1'!$J$30/SUM('Ver-Construção1'!$G$30:'Ver-Construção1'!$J$30))</f>
-        <v>#DIV/0!</v>
+        <v>0.4</v>
       </c>
       <c r="M32" s="7" t="s">
         <v>26</v>
@@ -5036,21 +5036,21 @@
       <c r="A33" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="B33" s="9" t="str">
+      <c r="B33" s="9">
         <f>('Ver-Construção1'!$G$36/SUM('Ver-Construção1'!$G$36:'Ver-Construção1'!$J$36))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C33" s="9" t="str">
+        <v>0.6666666667</v>
+      </c>
+      <c r="C33" s="9">
         <f>('Ver-Construção1'!$H$36/SUM('Ver-Construção1'!$G$36:'Ver-Construção1'!$J$36))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D33" s="9" t="str">
+        <v>0.3333333333</v>
+      </c>
+      <c r="D33" s="9">
         <f>('Ver-Construção1'!$I$36/SUM('Ver-Construção1'!$G$36:'Ver-Construção1'!$J$36))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E33" s="9" t="str">
+        <v>0</v>
+      </c>
+      <c r="E33" s="9">
         <f>('Ver-Construção1'!$J$36/SUM('Ver-Construção1'!$G$36:'Ver-Construção1'!$J$36))</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="M33" s="7" t="s">
         <v>27</v>
@@ -5076,21 +5076,21 @@
       <c r="A34" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="B34" s="9" t="str">
+      <c r="B34" s="9">
         <f>('Ver-Construção1'!$G$41/SUM('Ver-Construção1'!$G$41:'Ver-Construção1'!$J$41))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C34" s="9" t="str">
+        <v>0.5</v>
+      </c>
+      <c r="C34" s="9">
         <f>('Ver-Construção1'!$H$41/SUM('Ver-Construção1'!$G$41:'Ver-Construção1'!$J$41))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D34" s="9" t="str">
+        <v>0</v>
+      </c>
+      <c r="D34" s="9">
         <f>('Ver-Construção1'!$I$41/SUM('Ver-Construção1'!$G$41:'Ver-Construção1'!$J$41))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E34" s="9" t="str">
+        <v>0</v>
+      </c>
+      <c r="E34" s="9">
         <f>('Ver-Construção1'!$J$41/SUM('Ver-Construção1'!$G$41:'Ver-Construção1'!$J$41))</f>
-        <v>#DIV/0!</v>
+        <v>0.5</v>
       </c>
       <c r="M34" s="7" t="s">
         <v>28</v>
@@ -8575,7 +8575,7 @@
       <c r="E2" s="15"/>
       <c r="F2" s="16">
         <f>COUNTIF(D5:D41,"Sim")/(COUNTA(D5:D42)-COUNTIF(D5:D42,"NA"))</f>
-        <v>0.8181818182</v>
+        <v>0.8636363636</v>
       </c>
     </row>
     <row r="3" ht="18.75" customHeight="1">
@@ -9089,11 +9089,11 @@
       <c r="F29" s="30"/>
       <c r="G29" s="7">
         <f>COUNTIF(D29:D34,"Sim")</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H29" s="7">
         <f>COUNTIF(D29:D34,"Parcialmente")</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I29" s="7">
         <f>COUNTIF(D29:D34,"Não")</f>
@@ -9113,7 +9113,7 @@
         <v>93</v>
       </c>
       <c r="D30" s="45" t="s">
-        <v>72</v>
+        <v>46</v>
       </c>
       <c r="E30" s="30"/>
       <c r="F30" s="30"/>
@@ -10926,9 +10926,9 @@
         <v>31</v>
       </c>
       <c r="E2" s="15"/>
-      <c r="F2" s="16" t="str">
+      <c r="F2" s="16">
         <f>COUNTIF(D5:D42,"Sim")/(COUNTA(D5:D41)-COUNTIF(D5:D41,"NA"))</f>
-        <v>#DIV/0!</v>
+        <v>0.8695652174</v>
       </c>
     </row>
     <row r="3" ht="18.75" customHeight="1">
@@ -10983,12 +10983,14 @@
       <c r="C6" s="30" t="s">
         <v>73</v>
       </c>
-      <c r="D6" s="31"/>
+      <c r="D6" s="45" t="s">
+        <v>46</v>
+      </c>
       <c r="E6" s="30"/>
       <c r="F6" s="30"/>
       <c r="G6" s="7">
         <f>COUNTIF(D6,"Sim")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H6" s="7">
         <f>COUNTIF(D6,"Parcialmente")</f>
@@ -11021,12 +11023,14 @@
       <c r="C8" s="30" t="s">
         <v>74</v>
       </c>
-      <c r="D8" s="31"/>
+      <c r="D8" s="45" t="s">
+        <v>46</v>
+      </c>
       <c r="E8" s="30"/>
       <c r="F8" s="30"/>
       <c r="G8" s="7">
         <f>COUNTIF(D8,"Sim")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H8" s="7">
         <f>COUNTIF(D8,"Parcialmente")</f>
@@ -11075,12 +11079,14 @@
       <c r="C10" s="30" t="s">
         <v>76</v>
       </c>
-      <c r="D10" s="31"/>
+      <c r="D10" s="45" t="s">
+        <v>46</v>
+      </c>
       <c r="E10" s="30"/>
       <c r="F10" s="30"/>
       <c r="G10" s="7">
         <f>COUNTIF(D10:D12,"Sim")</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H10" s="7">
         <f>COUNTIF(D10:D12,"Parcialmente")</f>
@@ -11103,7 +11109,9 @@
       <c r="C11" s="30" t="s">
         <v>100</v>
       </c>
-      <c r="D11" s="31"/>
+      <c r="D11" s="45" t="s">
+        <v>46</v>
+      </c>
       <c r="E11" s="30"/>
       <c r="F11" s="30"/>
     </row>
@@ -11115,7 +11123,9 @@
       <c r="C12" s="30" t="s">
         <v>78</v>
       </c>
-      <c r="D12" s="31"/>
+      <c r="D12" s="45" t="s">
+        <v>46</v>
+      </c>
       <c r="E12" s="30"/>
       <c r="F12" s="30"/>
     </row>
@@ -11179,12 +11189,14 @@
       <c r="C16" s="30" t="s">
         <v>101</v>
       </c>
-      <c r="D16" s="31"/>
+      <c r="D16" s="45" t="s">
+        <v>46</v>
+      </c>
       <c r="E16" s="30"/>
       <c r="F16" s="30"/>
       <c r="G16" s="7">
         <f>COUNTIF(D16,"Sim")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H16" s="7">
         <f>COUNTIF(D16,"Parcialmente")</f>
@@ -11219,16 +11231,18 @@
       <c r="C18" s="30" t="s">
         <v>102</v>
       </c>
-      <c r="D18" s="31"/>
+      <c r="D18" s="45" t="s">
+        <v>46</v>
+      </c>
       <c r="E18" s="30"/>
       <c r="F18" s="30"/>
       <c r="G18" s="7">
         <f>COUNTIF(D18:D22,"Sim")</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H18" s="7">
         <f>COUNTIF(D18:D22,"Parcialmente")</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I18" s="7">
         <f>COUNTIF(D18:D22,"Não")</f>
@@ -11247,7 +11261,9 @@
       <c r="C19" s="30" t="s">
         <v>87</v>
       </c>
-      <c r="D19" s="31"/>
+      <c r="D19" s="45" t="s">
+        <v>46</v>
+      </c>
       <c r="E19" s="30"/>
       <c r="F19" s="30"/>
     </row>
@@ -11259,7 +11275,9 @@
       <c r="C20" s="30" t="s">
         <v>88</v>
       </c>
-      <c r="D20" s="31"/>
+      <c r="D20" s="45" t="s">
+        <v>72</v>
+      </c>
       <c r="E20" s="30"/>
       <c r="F20" s="30"/>
     </row>
@@ -11271,7 +11289,9 @@
       <c r="C21" s="30" t="s">
         <v>89</v>
       </c>
-      <c r="D21" s="31"/>
+      <c r="D21" s="45" t="s">
+        <v>46</v>
+      </c>
       <c r="E21" s="30"/>
       <c r="F21" s="30"/>
     </row>
@@ -11283,7 +11303,9 @@
       <c r="C22" s="30" t="s">
         <v>90</v>
       </c>
-      <c r="D22" s="31"/>
+      <c r="D22" s="45" t="s">
+        <v>72</v>
+      </c>
       <c r="E22" s="30"/>
       <c r="F22" s="30"/>
     </row>
@@ -11307,12 +11329,14 @@
       <c r="C24" s="34" t="s">
         <v>45</v>
       </c>
-      <c r="D24" s="31"/>
+      <c r="D24" s="45" t="s">
+        <v>46</v>
+      </c>
       <c r="E24" s="30"/>
       <c r="F24" s="30"/>
       <c r="G24" s="7">
         <f>COUNTIF(D24:D28,"Sim")</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H24" s="7">
         <f>COUNTIF(D24:D28,"Parcialmente")</f>
@@ -11335,7 +11359,9 @@
       <c r="C25" s="30" t="s">
         <v>104</v>
       </c>
-      <c r="D25" s="31"/>
+      <c r="D25" s="45" t="s">
+        <v>46</v>
+      </c>
       <c r="E25" s="30"/>
       <c r="F25" s="30"/>
     </row>
@@ -11347,7 +11373,9 @@
       <c r="C26" s="30" t="s">
         <v>105</v>
       </c>
-      <c r="D26" s="31"/>
+      <c r="D26" s="45" t="s">
+        <v>46</v>
+      </c>
       <c r="E26" s="30"/>
       <c r="F26" s="30"/>
     </row>
@@ -11359,7 +11387,9 @@
       <c r="C27" s="30" t="s">
         <v>106</v>
       </c>
-      <c r="D27" s="31"/>
+      <c r="D27" s="45" t="s">
+        <v>46</v>
+      </c>
       <c r="E27" s="30"/>
       <c r="F27" s="30"/>
     </row>
@@ -11371,7 +11401,9 @@
       <c r="C28" s="30" t="s">
         <v>107</v>
       </c>
-      <c r="D28" s="31"/>
+      <c r="D28" s="45" t="s">
+        <v>46</v>
+      </c>
       <c r="E28" s="30"/>
       <c r="F28" s="30"/>
     </row>
@@ -11395,12 +11427,14 @@
       <c r="C30" s="30" t="s">
         <v>92</v>
       </c>
-      <c r="D30" s="31"/>
+      <c r="D30" s="45" t="s">
+        <v>46</v>
+      </c>
       <c r="E30" s="30"/>
       <c r="F30" s="30"/>
       <c r="G30" s="7">
         <f>COUNTIF(D30:D34,"Sim")</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H30" s="7">
         <f>COUNTIF(D30:D34,"Parcialmente")</f>
@@ -11412,7 +11446,7 @@
       </c>
       <c r="J30" s="7">
         <f>COUNTIF(D30:D34,"NA")</f>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="31" ht="18.75" customHeight="1">
@@ -11423,7 +11457,9 @@
       <c r="C31" s="30" t="s">
         <v>108</v>
       </c>
-      <c r="D31" s="31"/>
+      <c r="D31" s="45" t="s">
+        <v>46</v>
+      </c>
       <c r="E31" s="30"/>
       <c r="F31" s="30"/>
     </row>
@@ -11435,7 +11471,9 @@
       <c r="C32" s="30" t="s">
         <v>109</v>
       </c>
-      <c r="D32" s="31"/>
+      <c r="D32" s="45" t="s">
+        <v>46</v>
+      </c>
       <c r="E32" s="30"/>
       <c r="F32" s="30"/>
     </row>
@@ -11447,7 +11485,9 @@
       <c r="C33" s="30" t="s">
         <v>96</v>
       </c>
-      <c r="D33" s="31"/>
+      <c r="D33" s="45" t="s">
+        <v>43</v>
+      </c>
       <c r="E33" s="30"/>
       <c r="F33" s="30"/>
     </row>
@@ -11459,7 +11499,9 @@
       <c r="C34" s="30" t="s">
         <v>97</v>
       </c>
-      <c r="D34" s="31"/>
+      <c r="D34" s="45" t="s">
+        <v>43</v>
+      </c>
       <c r="E34" s="30"/>
       <c r="F34" s="30"/>
     </row>
@@ -11483,16 +11525,18 @@
       <c r="C36" s="30" t="s">
         <v>69</v>
       </c>
-      <c r="D36" s="31"/>
+      <c r="D36" s="45" t="s">
+        <v>46</v>
+      </c>
       <c r="E36" s="30"/>
       <c r="F36" s="30"/>
       <c r="G36" s="7">
         <f>COUNTIF(D36:D38,"Sim")</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H36" s="7">
         <f>COUNTIF(D36:D38,"Parcialmente")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I36" s="7">
         <f>COUNTIF(D36:D38,"Não")</f>
@@ -11511,7 +11555,9 @@
       <c r="C37" s="30" t="s">
         <v>70</v>
       </c>
-      <c r="D37" s="31"/>
+      <c r="D37" s="45" t="s">
+        <v>46</v>
+      </c>
       <c r="E37" s="30"/>
       <c r="F37" s="30"/>
     </row>
@@ -11523,7 +11569,9 @@
       <c r="C38" s="30" t="s">
         <v>71</v>
       </c>
-      <c r="D38" s="31"/>
+      <c r="D38" s="45" t="s">
+        <v>72</v>
+      </c>
       <c r="E38" s="30"/>
       <c r="F38" s="30"/>
     </row>
@@ -11533,7 +11581,9 @@
       <c r="C39" s="30" t="s">
         <v>110</v>
       </c>
-      <c r="D39" s="31"/>
+      <c r="D39" s="45" t="s">
+        <v>72</v>
+      </c>
       <c r="E39" s="30"/>
       <c r="F39" s="30"/>
     </row>
@@ -11555,12 +11605,14 @@
       <c r="C41" s="30" t="s">
         <v>98</v>
       </c>
-      <c r="D41" s="31"/>
+      <c r="D41" s="45" t="s">
+        <v>43</v>
+      </c>
       <c r="E41" s="30"/>
       <c r="F41" s="30"/>
       <c r="G41" s="7">
         <f>COUNTIF(D41:D42,"Sim")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H41" s="7">
         <f>COUNTIF(D41:D42,"Parcialmente")</f>
@@ -11572,7 +11624,7 @@
       </c>
       <c r="J41" s="7">
         <f>COUNTIF(D41:D42,"NA")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="42" ht="18.75" customHeight="1">
@@ -11583,7 +11635,9 @@
       <c r="C42" s="30" t="s">
         <v>99</v>
       </c>
-      <c r="D42" s="31"/>
+      <c r="D42" s="45" t="s">
+        <v>46</v>
+      </c>
       <c r="E42" s="30"/>
       <c r="F42" s="30"/>
     </row>

</xml_diff>

<commit_message>
Atualizacao da planilha de planejamento e da planilha de checklist apos realizacao da fase de transicao e adicao do do diagrama de deployment
</commit_message>
<xml_diff>
--- a/SGB/6.Gerenciamento de Projeto/SGB - Checklist Verificacao de Projeto.xlsx
+++ b/SGB/6.Gerenciamento de Projeto/SGB - Checklist Verificacao de Projeto.xlsx
@@ -241,7 +241,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="118">
   <si>
     <t>IAP - Indicador de Aderência ao Processo (70% a 100%)</t>
   </si>
@@ -1072,11 +1072,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="1277942220"/>
-        <c:axId val="765381546"/>
+        <c:axId val="532273003"/>
+        <c:axId val="1147928154"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1277942220"/>
+        <c:axId val="532273003"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1128,10 +1128,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="765381546"/>
+        <c:crossAx val="1147928154"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="765381546"/>
+        <c:axId val="1147928154"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1195,7 +1195,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1277942220"/>
+        <c:crossAx val="532273003"/>
       </c:valAx>
     </c:plotArea>
     <c:plotVisOnly val="1"/>
@@ -1350,11 +1350,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="8186131"/>
-        <c:axId val="820519570"/>
+        <c:axId val="1718688859"/>
+        <c:axId val="497023869"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="8186131"/>
+        <c:axId val="1718688859"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1406,10 +1406,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="820519570"/>
+        <c:crossAx val="497023869"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="820519570"/>
+        <c:axId val="497023869"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1473,7 +1473,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="8186131"/>
+        <c:crossAx val="1718688859"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -1646,11 +1646,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="934834915"/>
-        <c:axId val="297186432"/>
+        <c:axId val="1109365861"/>
+        <c:axId val="1115475371"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="934834915"/>
+        <c:axId val="1109365861"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1702,10 +1702,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="297186432"/>
+        <c:crossAx val="1115475371"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="297186432"/>
+        <c:axId val="1115475371"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1769,7 +1769,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="934834915"/>
+        <c:crossAx val="1109365861"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -1950,11 +1950,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="736625280"/>
-        <c:axId val="515221719"/>
+        <c:axId val="383882468"/>
+        <c:axId val="840278579"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="736625280"/>
+        <c:axId val="383882468"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2006,10 +2006,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="515221719"/>
+        <c:crossAx val="840278579"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="515221719"/>
+        <c:axId val="840278579"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2064,7 +2064,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="736625280"/>
+        <c:crossAx val="383882468"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -2133,6 +2133,16 @@
               <c:f>Detalhado!$N$24</c:f>
             </c:strRef>
           </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
           <c:cat>
             <c:strRef>
               <c:f>Detalhado!$M$25:$M$37</c:f>
@@ -2153,6 +2163,16 @@
               <c:f>Detalhado!$O$24</c:f>
             </c:strRef>
           </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
           <c:cat>
             <c:strRef>
               <c:f>Detalhado!$M$25:$M$37</c:f>
@@ -2173,6 +2193,16 @@
               <c:f>Detalhado!$P$24</c:f>
             </c:strRef>
           </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
           <c:cat>
             <c:strRef>
               <c:f>Detalhado!$M$25:$M$37</c:f>
@@ -2193,6 +2223,16 @@
               <c:f>Detalhado!$Q$24</c:f>
             </c:strRef>
           </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
           <c:cat>
             <c:strRef>
               <c:f>Detalhado!$M$25:$M$37</c:f>
@@ -2205,11 +2245,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="2096883095"/>
-        <c:axId val="665270780"/>
+        <c:axId val="247294614"/>
+        <c:axId val="1227952937"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2096883095"/>
+        <c:axId val="247294614"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2261,22 +2301,65 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="665270780"/>
+        <c:crossAx val="1227952937"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="665270780"/>
+        <c:axId val="1227952937"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:rPr>
+                  <a:t/>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
+          <a:ln/>
         </c:spPr>
-        <c:crossAx val="2096883095"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="247294614"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -2700,16 +2783,16 @@
       </c>
       <c r="B5" s="5">
         <f>'Ver-Construção1'!$F$2</f>
-        <v>0.8695652174</v>
+        <v>0.9130434783</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="5" t="str">
+      <c r="B6" s="5">
         <f>'Ver-Transição1'!$F$2</f>
-        <v>#DIV/0!</v>
+        <v>0.9166666667</v>
       </c>
     </row>
     <row r="8">
@@ -4735,21 +4818,21 @@
       <c r="M25" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="N25" s="9" t="str">
+      <c r="N25" s="9">
         <f>('Ver-Transição1'!$G$6/SUM('Ver-Transição1'!$G$6:'Ver-Transição1'!$J$6))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O25" s="9" t="str">
+        <v>1</v>
+      </c>
+      <c r="O25" s="9">
         <f>('Ver-Transição1'!$H$6/SUM('Ver-Transição1'!$G$6:'Ver-Transição1'!$J$6))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P25" s="9" t="str">
+        <v>0</v>
+      </c>
+      <c r="P25" s="9">
         <f>('Ver-Transição1'!$I$6/SUM('Ver-Transição1'!$G$6:'Ver-Transição1'!$J$6))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q25" s="9" t="str">
+        <v>0</v>
+      </c>
+      <c r="Q25" s="9">
         <f>('Ver-Transição1'!$J$6/SUM('Ver-Transição1'!$G$6:'Ver-Transição1'!$J$6))</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" ht="15.75" customHeight="1">
@@ -4775,21 +4858,21 @@
       <c r="M26" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="N26" s="9" t="str">
+      <c r="N26" s="9">
         <f>('Ver-Transição1'!$G$8/SUM('Ver-Transição1'!$G$8:'Ver-Transição1'!$J$8))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O26" s="9" t="str">
+        <v>1</v>
+      </c>
+      <c r="O26" s="9">
         <f>('Ver-Transição1'!$H$8/SUM('Ver-Transição1'!$G$8:'Ver-Transição1'!$J$8))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P26" s="9" t="str">
+        <v>0</v>
+      </c>
+      <c r="P26" s="9">
         <f>('Ver-Transição1'!$I$8/SUM('Ver-Transição1'!$G$8:'Ver-Transição1'!$J$8))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q26" s="9" t="str">
+        <v>0</v>
+      </c>
+      <c r="Q26" s="9">
         <f>('Ver-Transição1'!$J$8/SUM('Ver-Transição1'!$G$8:'Ver-Transição1'!$J$8))</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" ht="15.75" customHeight="1">
@@ -4815,21 +4898,21 @@
       <c r="M27" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="N27" s="9" t="str">
+      <c r="N27" s="9">
         <f>('Ver-Transição1'!$G$10/SUM('Ver-Transição1'!$G$10:'Ver-Transição1'!$J$10))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O27" s="9" t="str">
+        <v>1</v>
+      </c>
+      <c r="O27" s="9">
         <f>('Ver-Transição1'!$H$10/SUM('Ver-Transição1'!$G$10:'Ver-Transição1'!$J$10))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P27" s="9" t="str">
+        <v>0</v>
+      </c>
+      <c r="P27" s="9">
         <f>('Ver-Transição1'!$I$10/SUM('Ver-Transição1'!$G$10:'Ver-Transição1'!$J$10))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q27" s="9" t="str">
+        <v>0</v>
+      </c>
+      <c r="Q27" s="9">
         <f>('Ver-Transição1'!$J$10/SUM('Ver-Transição1'!$G$10:'Ver-Transição1'!$J$10))</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" ht="15.75" customHeight="1">
@@ -4855,21 +4938,21 @@
       <c r="M28" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="N28" s="9" t="str">
+      <c r="N28" s="9">
         <f>('Ver-Transição1'!$G$14/SUM('Ver-Transição1'!$G$14:'Ver-Transição1'!$J$14))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O28" s="9" t="str">
+        <v>0</v>
+      </c>
+      <c r="O28" s="9">
         <f>('Ver-Transição1'!$H$14/SUM('Ver-Transição1'!$G$14:'Ver-Transição1'!$J$14))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P28" s="9" t="str">
+        <v>0</v>
+      </c>
+      <c r="P28" s="9">
         <f>('Ver-Transição1'!$I$14/SUM('Ver-Transição1'!$G$14:'Ver-Transição1'!$J$14))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q28" s="9" t="str">
+        <v>0</v>
+      </c>
+      <c r="Q28" s="9">
         <f>('Ver-Transição1'!$J$14/SUM('Ver-Transição1'!$G$14:'Ver-Transição1'!$J$14))</f>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" ht="15.75" customHeight="1">
@@ -4918,11 +5001,11 @@
       </c>
       <c r="B30" s="9">
         <f>('Ver-Construção1'!$G$18/SUM('Ver-Construção1'!$G$18:'Ver-Construção1'!$J$18))</f>
-        <v>0.6</v>
+        <v>0.8</v>
       </c>
       <c r="C30" s="9">
         <f>('Ver-Construção1'!$H$18/SUM('Ver-Construção1'!$G$18:'Ver-Construção1'!$J$18))</f>
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
       <c r="D30" s="9">
         <f>('Ver-Construção1'!$I$18/SUM('Ver-Construção1'!$G$18:'Ver-Construção1'!$J$18))</f>
@@ -4935,21 +5018,21 @@
       <c r="M30" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="N30" s="9" t="str">
+      <c r="N30" s="9">
         <f>('Ver-Transição1'!$G$16/SUM('Ver-Transição1'!$G$16:'Ver-Transição1'!$J$16))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O30" s="9" t="str">
+        <v>1</v>
+      </c>
+      <c r="O30" s="9">
         <f>('Ver-Transição1'!$H$16/SUM('Ver-Transição1'!$G$16:'Ver-Transição1'!$J$16))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P30" s="9" t="str">
+        <v>0</v>
+      </c>
+      <c r="P30" s="9">
         <f>('Ver-Transição1'!$I$16/SUM('Ver-Transição1'!$G$16:'Ver-Transição1'!$J$16))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q30" s="9" t="str">
+        <v>0</v>
+      </c>
+      <c r="Q30" s="9">
         <f>('Ver-Transição1'!$J$16/SUM('Ver-Transição1'!$G$16:'Ver-Transição1'!$J$16))</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" ht="15.75" customHeight="1">
@@ -4975,21 +5058,21 @@
       <c r="M31" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="N31" s="9" t="str">
+      <c r="N31" s="9">
         <f>('Ver-Transição1'!$G$18/SUM('Ver-Transição1'!$G$18:'Ver-Transição1'!$J$18))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O31" s="9" t="str">
+        <v>1</v>
+      </c>
+      <c r="O31" s="9">
         <f>('Ver-Transição1'!$H$18/SUM('Ver-Transição1'!$G$18:'Ver-Transição1'!$J$18))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P31" s="9" t="str">
+        <v>0</v>
+      </c>
+      <c r="P31" s="9">
         <f>('Ver-Transição1'!$I$18/SUM('Ver-Transição1'!$G$18:'Ver-Transição1'!$J$18))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q31" s="9" t="str">
+        <v>0</v>
+      </c>
+      <c r="Q31" s="9">
         <f>('Ver-Transição1'!$J$18/SUM('Ver-Transição1'!$G$18:'Ver-Transição1'!$J$18))</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32" ht="15.75" customHeight="1">
@@ -5015,21 +5098,21 @@
       <c r="M32" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="N32" s="9" t="str">
+      <c r="N32" s="9">
         <f>('Ver-Transição1'!$G$23/SUM('Ver-Transição1'!$G$23:'Ver-Transição1'!$J$23))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O32" s="9" t="str">
+        <v>1</v>
+      </c>
+      <c r="O32" s="9">
         <f>('Ver-Transição1'!$H$23/SUM('Ver-Transição1'!$G$23:'Ver-Transição1'!$J$23))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P32" s="9" t="str">
+        <v>0</v>
+      </c>
+      <c r="P32" s="9">
         <f>('Ver-Transição1'!$I$23/SUM('Ver-Transição1'!$G$23:'Ver-Transição1'!$J$23))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q32" s="9" t="str">
+        <v>0</v>
+      </c>
+      <c r="Q32" s="9">
         <f>('Ver-Transição1'!$J$23/SUM('Ver-Transição1'!$G$23:'Ver-Transição1'!$J$23))</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33" ht="15.75" customHeight="1">
@@ -5055,21 +5138,21 @@
       <c r="M33" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="N33" s="9" t="str">
+      <c r="N33" s="9">
         <f>('Ver-Transição1'!$G$26/SUM('Ver-Transição1'!$G$26:'Ver-Transição1'!$J$26))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O33" s="9" t="str">
+        <v>1</v>
+      </c>
+      <c r="O33" s="9">
         <f>('Ver-Transição1'!$H$26/SUM('Ver-Transição1'!$G$26:'Ver-Transição1'!$J$26))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P33" s="9" t="str">
+        <v>0</v>
+      </c>
+      <c r="P33" s="9">
         <f>('Ver-Transição1'!$I$26/SUM('Ver-Transição1'!$G$26:'Ver-Transição1'!$J$26))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q33" s="9" t="str">
+        <v>0</v>
+      </c>
+      <c r="Q33" s="9">
         <f>('Ver-Transição1'!$J$26/SUM('Ver-Transição1'!$G$26:'Ver-Transição1'!$J$26))</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34" ht="15.75" customHeight="1">
@@ -5095,84 +5178,84 @@
       <c r="M34" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="N34" s="8" t="str">
+      <c r="N34" s="8">
         <f>('Ver-Transição1'!$G$29/SUM('Ver-Transição1'!$G$29:'Ver-Transição1'!$J$29))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O34" s="9" t="str">
+        <v>1</v>
+      </c>
+      <c r="O34" s="9">
         <f>('Ver-Transição1'!$H$29/SUM('Ver-Transição1'!$G$29:'Ver-Transição1'!$J$29))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P34" s="9" t="str">
+        <v>0</v>
+      </c>
+      <c r="P34" s="9">
         <f>('Ver-Transição1'!$I$29/SUM('Ver-Transição1'!$G$29:'Ver-Transição1'!$J$29))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q34" s="9" t="str">
+        <v>0</v>
+      </c>
+      <c r="Q34" s="9">
         <f>('Ver-Transição1'!$J$29/SUM('Ver-Transição1'!$G$29:'Ver-Transição1'!$J$29))</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35" ht="15.75" customHeight="1">
       <c r="M35" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="N35" s="9" t="str">
+      <c r="N35" s="9">
         <f>('Ver-Transição1'!$G$31/SUM('Ver-Transição1'!$G$31:'Ver-Transição1'!$J$31))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O35" s="9" t="str">
+        <v>0.6</v>
+      </c>
+      <c r="O35" s="9">
         <f>('Ver-Transição1'!$H$31/SUM('Ver-Transição1'!$G$31:'Ver-Transição1'!$J$31))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P35" s="9" t="str">
+        <v>0</v>
+      </c>
+      <c r="P35" s="9">
         <f>('Ver-Transição1'!$I$31/SUM('Ver-Transição1'!$G$31:'Ver-Transição1'!$J$31))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q35" s="9" t="str">
+        <v>0</v>
+      </c>
+      <c r="Q35" s="9">
         <f>('Ver-Transição1'!$J$31/SUM('Ver-Transição1'!$G$31:'Ver-Transição1'!$J$31))</f>
-        <v>#DIV/0!</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="36" ht="15.75" customHeight="1">
       <c r="M36" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="N36" s="9" t="str">
+      <c r="N36" s="9">
         <f>('Ver-Transição1'!$G$37/SUM('Ver-Transição1'!$G$37:'Ver-Transição1'!$J$37))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O36" s="9" t="str">
+        <v>0.6666666667</v>
+      </c>
+      <c r="O36" s="9">
         <f>('Ver-Transição1'!$H$37/SUM('Ver-Transição1'!$G$37:'Ver-Transição1'!$J$37))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P36" s="9" t="str">
+        <v>0.3333333333</v>
+      </c>
+      <c r="P36" s="9">
         <f>('Ver-Transição1'!$I$37/SUM('Ver-Transição1'!$G$37:'Ver-Transição1'!$J$37))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q36" s="9" t="str">
+        <v>0</v>
+      </c>
+      <c r="Q36" s="9">
         <f>('Ver-Transição1'!$J$37/SUM('Ver-Transição1'!$G$37:'Ver-Transição1'!$J$37))</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37" ht="15.75" customHeight="1">
       <c r="M37" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="N37" s="9" t="str">
+      <c r="N37" s="9">
         <f>('Ver-Transição1'!$G$42/SUM('Ver-Transição1'!$G$42:'Ver-Transição1'!$J$42))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O37" s="9" t="str">
+        <v>1</v>
+      </c>
+      <c r="O37" s="9">
         <f>('Ver-Transição1'!$H$42/SUM('Ver-Transição1'!$G$42:'Ver-Transição1'!$J$42))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P37" s="9" t="str">
+        <v>0</v>
+      </c>
+      <c r="P37" s="9">
         <f>('Ver-Transição1'!$I$42/SUM('Ver-Transição1'!$G$42:'Ver-Transição1'!$J$42))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q37" s="9" t="str">
+        <v>0</v>
+      </c>
+      <c r="Q37" s="9">
         <f>('Ver-Transição1'!$J$42/SUM('Ver-Transição1'!$G$42:'Ver-Transição1'!$J$42))</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38" ht="15.75" customHeight="1"/>
@@ -10928,7 +11011,7 @@
       <c r="E2" s="15"/>
       <c r="F2" s="16">
         <f>COUNTIF(D5:D42,"Sim")/(COUNTA(D5:D41)-COUNTIF(D5:D41,"NA"))</f>
-        <v>0.8695652174</v>
+        <v>0.9130434783</v>
       </c>
     </row>
     <row r="3" ht="18.75" customHeight="1">
@@ -11238,11 +11321,11 @@
       <c r="F18" s="30"/>
       <c r="G18" s="7">
         <f>COUNTIF(D18:D22,"Sim")</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H18" s="7">
         <f>COUNTIF(D18:D22,"Parcialmente")</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I18" s="7">
         <f>COUNTIF(D18:D22,"Não")</f>
@@ -11304,7 +11387,7 @@
         <v>90</v>
       </c>
       <c r="D22" s="45" t="s">
-        <v>72</v>
+        <v>46</v>
       </c>
       <c r="E22" s="30"/>
       <c r="F22" s="30"/>
@@ -13248,9 +13331,9 @@
         <v>31</v>
       </c>
       <c r="E2" s="15"/>
-      <c r="F2" s="16" t="str">
+      <c r="F2" s="16">
         <f>COUNTIF(D5:D43,"Sim")/(COUNTA(D5:D43)-COUNTIF(D5:D43,"NA"))</f>
-        <v>#DIV/0!</v>
+        <v>0.9166666667</v>
       </c>
     </row>
     <row r="3" ht="18.75" customHeight="1">
@@ -13305,12 +13388,14 @@
       <c r="C6" s="30" t="s">
         <v>73</v>
       </c>
-      <c r="D6" s="31"/>
+      <c r="D6" s="45" t="s">
+        <v>46</v>
+      </c>
       <c r="E6" s="30"/>
       <c r="F6" s="30"/>
       <c r="G6" s="7">
         <f>COUNTIF(D6,"Sim")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H6" s="7">
         <f>COUNTIF(D6,"Parcialmente")</f>
@@ -13343,12 +13428,14 @@
       <c r="C8" s="30" t="s">
         <v>74</v>
       </c>
-      <c r="D8" s="31"/>
+      <c r="D8" s="45" t="s">
+        <v>46</v>
+      </c>
       <c r="E8" s="30"/>
       <c r="F8" s="30"/>
       <c r="G8" s="7">
         <f>COUNTIF(D8,"Sim")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H8" s="7">
         <f>COUNTIF(D8,"Parcialmente")</f>
@@ -13397,12 +13484,14 @@
       <c r="C10" s="30" t="s">
         <v>76</v>
       </c>
-      <c r="D10" s="31"/>
+      <c r="D10" s="45" t="s">
+        <v>46</v>
+      </c>
       <c r="E10" s="30"/>
       <c r="F10" s="30"/>
       <c r="G10" s="7">
         <f>COUNTIF(D10:D12,"Sim")</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H10" s="7">
         <f>COUNTIF(D10:D12,"Parcialmente")</f>
@@ -13425,7 +13514,9 @@
       <c r="C11" s="30" t="s">
         <v>100</v>
       </c>
-      <c r="D11" s="31"/>
+      <c r="D11" s="45" t="s">
+        <v>46</v>
+      </c>
       <c r="E11" s="30"/>
       <c r="F11" s="30"/>
     </row>
@@ -13437,7 +13528,9 @@
       <c r="C12" s="30" t="s">
         <v>78</v>
       </c>
-      <c r="D12" s="31"/>
+      <c r="D12" s="45" t="s">
+        <v>46</v>
+      </c>
       <c r="E12" s="30"/>
       <c r="F12" s="30"/>
     </row>
@@ -13459,7 +13552,9 @@
       <c r="C14" s="30" t="s">
         <v>80</v>
       </c>
-      <c r="D14" s="31"/>
+      <c r="D14" s="45" t="s">
+        <v>43</v>
+      </c>
       <c r="E14" s="30"/>
       <c r="F14" s="30"/>
       <c r="G14" s="7">
@@ -13476,7 +13571,7 @@
       </c>
       <c r="J14" s="7">
         <f>COUNTIF(D14,"NA")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" ht="15.0" customHeight="1">
@@ -13499,12 +13594,14 @@
       <c r="C16" s="30" t="s">
         <v>101</v>
       </c>
-      <c r="D16" s="31"/>
+      <c r="D16" s="45" t="s">
+        <v>46</v>
+      </c>
       <c r="E16" s="30"/>
       <c r="F16" s="30"/>
       <c r="G16" s="7">
         <f>COUNTIF(D16,"Sim")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H16" s="7">
         <f>COUNTIF(D16,"Parcialmente")</f>
@@ -13539,12 +13636,14 @@
       <c r="C18" s="30" t="s">
         <v>111</v>
       </c>
-      <c r="D18" s="31"/>
+      <c r="D18" s="45" t="s">
+        <v>46</v>
+      </c>
       <c r="E18" s="30"/>
       <c r="F18" s="30"/>
       <c r="G18" s="7">
         <f>COUNTIF(D18:D21,"Sim")</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H18" s="7">
         <f>COUNTIF(D18:D21,"Parcialmente")</f>
@@ -13567,7 +13666,9 @@
       <c r="C19" s="30" t="s">
         <v>112</v>
       </c>
-      <c r="D19" s="31"/>
+      <c r="D19" s="45" t="s">
+        <v>46</v>
+      </c>
       <c r="E19" s="30"/>
       <c r="F19" s="30"/>
     </row>
@@ -13579,7 +13680,9 @@
       <c r="C20" s="30" t="s">
         <v>88</v>
       </c>
-      <c r="D20" s="31"/>
+      <c r="D20" s="45" t="s">
+        <v>46</v>
+      </c>
       <c r="E20" s="30"/>
       <c r="F20" s="30"/>
     </row>
@@ -13591,7 +13694,9 @@
       <c r="C21" s="30" t="s">
         <v>113</v>
       </c>
-      <c r="D21" s="31"/>
+      <c r="D21" s="45" t="s">
+        <v>46</v>
+      </c>
       <c r="E21" s="30"/>
       <c r="F21" s="30"/>
     </row>
@@ -13615,12 +13720,14 @@
       <c r="C23" s="30" t="s">
         <v>114</v>
       </c>
-      <c r="D23" s="31"/>
+      <c r="D23" s="45" t="s">
+        <v>46</v>
+      </c>
       <c r="E23" s="30"/>
       <c r="F23" s="30"/>
       <c r="G23" s="7">
         <f>COUNTIF(D23:D24,"Sim")</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H23" s="7">
         <f>COUNTIF(D23:D24,"Parcialmente")</f>
@@ -13643,7 +13750,9 @@
       <c r="C24" s="30" t="s">
         <v>107</v>
       </c>
-      <c r="D24" s="31"/>
+      <c r="D24" s="45" t="s">
+        <v>46</v>
+      </c>
       <c r="E24" s="30"/>
       <c r="F24" s="30"/>
     </row>
@@ -13687,12 +13796,14 @@
       <c r="C26" s="34" t="s">
         <v>45</v>
       </c>
-      <c r="D26" s="31"/>
+      <c r="D26" s="45" t="s">
+        <v>46</v>
+      </c>
       <c r="E26" s="30"/>
       <c r="F26" s="30"/>
       <c r="G26" s="7">
         <f>COUNTIF(D26:D27,"Sim")</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H26" s="7">
         <f>COUNTIF(D26:D27,"Parcialmente")</f>
@@ -13731,7 +13842,9 @@
       <c r="C27" s="30" t="s">
         <v>116</v>
       </c>
-      <c r="D27" s="31"/>
+      <c r="D27" s="45" t="s">
+        <v>46</v>
+      </c>
       <c r="E27" s="30"/>
       <c r="F27" s="30"/>
       <c r="G27" s="35"/>
@@ -13773,12 +13886,14 @@
       <c r="C29" s="34" t="s">
         <v>45</v>
       </c>
-      <c r="D29" s="31"/>
+      <c r="D29" s="45" t="s">
+        <v>46</v>
+      </c>
       <c r="E29" s="30"/>
       <c r="F29" s="30"/>
       <c r="G29" s="7">
         <f>COUNTIF(D29,"Sim")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H29" s="7">
         <f>COUNTIF(D29,"Parcialmente")</f>
@@ -13813,12 +13928,14 @@
       <c r="C31" s="30" t="s">
         <v>92</v>
       </c>
-      <c r="D31" s="31"/>
+      <c r="D31" s="45" t="s">
+        <v>46</v>
+      </c>
       <c r="E31" s="30"/>
       <c r="F31" s="30"/>
       <c r="G31" s="7">
         <f>COUNTIF(D31:D35,"Sim")</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H31" s="7">
         <f>COUNTIF(D31:D35,"Parcialmente")</f>
@@ -13830,7 +13947,7 @@
       </c>
       <c r="J31" s="7">
         <f>COUNTIF(D31:D35,"NA")</f>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="32" ht="18.75" customHeight="1">
@@ -13841,7 +13958,9 @@
       <c r="C32" s="30" t="s">
         <v>108</v>
       </c>
-      <c r="D32" s="31"/>
+      <c r="D32" s="45" t="s">
+        <v>46</v>
+      </c>
       <c r="E32" s="30"/>
       <c r="F32" s="30"/>
     </row>
@@ -13853,7 +13972,9 @@
       <c r="C33" s="30" t="s">
         <v>109</v>
       </c>
-      <c r="D33" s="31"/>
+      <c r="D33" s="45" t="s">
+        <v>46</v>
+      </c>
       <c r="E33" s="30"/>
       <c r="F33" s="30"/>
     </row>
@@ -13865,7 +13986,9 @@
       <c r="C34" s="30" t="s">
         <v>117</v>
       </c>
-      <c r="D34" s="31"/>
+      <c r="D34" s="45" t="s">
+        <v>43</v>
+      </c>
       <c r="E34" s="30"/>
       <c r="F34" s="30"/>
     </row>
@@ -13877,7 +14000,9 @@
       <c r="C35" s="30" t="s">
         <v>97</v>
       </c>
-      <c r="D35" s="31"/>
+      <c r="D35" s="45" t="s">
+        <v>43</v>
+      </c>
       <c r="E35" s="30"/>
       <c r="F35" s="30"/>
     </row>
@@ -13901,16 +14026,18 @@
       <c r="C37" s="30" t="s">
         <v>69</v>
       </c>
-      <c r="D37" s="31"/>
+      <c r="D37" s="45" t="s">
+        <v>46</v>
+      </c>
       <c r="E37" s="30"/>
       <c r="F37" s="30"/>
       <c r="G37" s="7">
         <f>COUNTIF(D37:D39,"Sim")</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H37" s="7">
         <f>COUNTIF(D37:D39,"Parcialmente")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I37" s="7">
         <f>COUNTIF(D37:D39,"Não")</f>
@@ -13929,7 +14056,9 @@
       <c r="C38" s="30" t="s">
         <v>70</v>
       </c>
-      <c r="D38" s="31"/>
+      <c r="D38" s="45" t="s">
+        <v>46</v>
+      </c>
       <c r="E38" s="30"/>
       <c r="F38" s="30"/>
     </row>
@@ -13941,7 +14070,9 @@
       <c r="C39" s="30" t="s">
         <v>71</v>
       </c>
-      <c r="D39" s="31"/>
+      <c r="D39" s="45" t="s">
+        <v>72</v>
+      </c>
       <c r="E39" s="30"/>
       <c r="F39" s="30"/>
     </row>
@@ -13951,7 +14082,9 @@
       <c r="C40" s="30" t="s">
         <v>110</v>
       </c>
-      <c r="D40" s="31"/>
+      <c r="D40" s="45" t="s">
+        <v>72</v>
+      </c>
       <c r="E40" s="30"/>
       <c r="F40" s="30"/>
     </row>
@@ -13973,12 +14106,14 @@
       <c r="C42" s="30" t="s">
         <v>98</v>
       </c>
-      <c r="D42" s="31"/>
+      <c r="D42" s="45" t="s">
+        <v>46</v>
+      </c>
       <c r="E42" s="30"/>
       <c r="F42" s="30"/>
       <c r="G42" s="7">
         <f>COUNTIF(D42:D43,"Sim")</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H42" s="7">
         <f>COUNTIF(D42:D43,"Parcialmente")</f>
@@ -14001,7 +14136,9 @@
       <c r="C43" s="30" t="s">
         <v>99</v>
       </c>
-      <c r="D43" s="31"/>
+      <c r="D43" s="45" t="s">
+        <v>46</v>
+      </c>
       <c r="E43" s="30"/>
       <c r="F43" s="30"/>
     </row>

</xml_diff>